<commit_message>
Só para o Túlio pegar atualizado
</commit_message>
<xml_diff>
--- a/data/teacher/Aderci.xlsx
+++ b/data/teacher/Aderci.xlsx
@@ -510,22 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>['MEC-3B-Fresagem', -, -, -]</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -542,22 +542,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>['MEC-3B-Fresagem', -, -, -]</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -606,22 +606,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>['MEC-3B-Fresagem', -, -, -]</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -638,22 +638,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>['MEC-3B-Fresagem', -, -, -]</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>['MEC-2A-Tornearia', -, -, -]</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, -, 'MEC-3A-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, 'MEC-3A-Fresagem', -, -]</t>
         </is>
       </c>
     </row>
@@ -808,12 +808,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, -, 'MEC-3A-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, 'MEC-3A-Fresagem', -, -]</t>
         </is>
       </c>
     </row>
@@ -872,12 +872,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, -, 'MEC-3A-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, 'MEC-3A-Fresagem', 'MEC-2A-Tornearia', -]</t>
         </is>
       </c>
     </row>
@@ -904,12 +904,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, -, 'MEC-3A-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, 'MEC-3A-Fresagem', 'MEC-2A-Tornearia', -]</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, 'MEC-2A-Tornearia', -]</t>
         </is>
       </c>
     </row>
@@ -985,12 +985,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NB-Fresagem', -, -]</t>
+          <t>['MEC-2NA-Fresagem', -, -, 'MEC-2NA-CAD/CAM']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1000,12 +1000,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NA-CAD/CAM', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
         </is>
       </c>
     </row>
@@ -1017,12 +1017,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NB-Fresagem', -, -]</t>
+          <t>['MEC-2NA-Fresagem', -, -, 'MEC-2NA-CAD/CAM']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1032,12 +1032,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NA-CAD/CAM', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
         </is>
       </c>
     </row>
@@ -1049,12 +1049,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NB-Fresagem', -, -]</t>
+          <t>['MEC-2NA-Fresagem', -, -, 'MEC-2NA-CAD/CAM']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1064,12 +1064,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NA-CAD/CAM', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1081,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NB-Fresagem', -, -]</t>
+          <t>['MEC-2NA-Fresagem', -, -, 'MEC-2NA-CAD/CAM']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1096,12 +1096,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NA-CAD/CAM', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Funcioando com o ELM-2NA
</commit_message>
<xml_diff>
--- a/data/teacher/Aderci.xlsx
+++ b/data/teacher/Aderci.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3B-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>['MEC-3A-Fresagem', -, -, -]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>[-, -, 'MEC-2A-Tornearia', -]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
         </is>
       </c>
     </row>
@@ -808,12 +808,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>['MEC-3A-Fresagem', -, -, -]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>[-, -, 'MEC-2A-Tornearia', -]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
         </is>
       </c>
     </row>
@@ -872,12 +872,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>['MEC-3A-Fresagem', -, -, -]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>[-, -, 'MEC-2A-Tornearia', -]</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -904,12 +904,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>['MEC-3A-Fresagem', -, -, -]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>[-, -, 'MEC-2A-Tornearia', -]</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['MEC-3A-Fresagem', -, -, -]</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -985,22 +985,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>[-, -, -, 'MEC-2NA-Fresagem']</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>[-, -, -, 'MEC-2NA-CAD/CAM']</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[-, -, -, 'MEC-2NA-CAD/CAM']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>[-, -, -, 'MEC-2NB-Fresagem']</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1017,22 +1017,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-2NA-CAD/CAM']</t>
+          <t>[-, -, 'MEC-2NA-CAD/CAM', 'MEC-2NA-Fresagem']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>[-, -, -, 'MEC-2NB-Fresagem']</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1049,22 +1049,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-2NA-CAD/CAM']</t>
+          <t>[-, -, 'MEC-2NA-CAD/CAM', 'MEC-2NA-Fresagem']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>[-, -, -, 'MEC-2NB-Fresagem']</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1081,22 +1081,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-2NA-CAD/CAM']</t>
+          <t>[-, -, -, 'MEC-2NA-Fresagem']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>[-, -, -, 'MEC-2NB-Fresagem']</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, -]</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">

</xml_diff>

<commit_message>
Listas sem duplicação de professores
</commit_message>
<xml_diff>
--- a/data/teacher/Aderci.xlsx
+++ b/data/teacher/Aderci.xlsx
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3B-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3B-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3B-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3B-Fresagem', -, -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, 'MEC-3A-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, 'MEC-3A-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -862,12 +862,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['MEC-2A-Tornearia', -, 'MEC-3A-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-2A-Tornearia']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -894,7 +894,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -985,12 +985,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, 'MEC-2NA-CAD/CAM']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1017,12 +1017,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, 'MEC-2NA-CAD/CAM']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1049,12 +1049,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, 'MEC-2NA-CAD/CAM']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1081,12 +1081,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-2NB-Fresagem', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[-, 'MEC-2NA-Fresagem', -, 'MEC-2NA-CAD/CAM']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
Savesheet para diferentes bimestres
</commit_message>
<xml_diff>
--- a/data/teacher/Aderci.xlsx
+++ b/data/teacher/Aderci.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3B-Fresagem</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3B-Fresagem</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>MEC-3B-Fresagem</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3B-Fresagem']</t>
+          <t>MEC-3B-Fresagem</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3A-M. A. Comp; Cad / CAM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3A-M. A. Comp; Cad / CAM']</t>
+          <t>MEC-3A-Fresagem</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-M. A. Comp; Cad / CAM', -]</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['MEC-3A-Fresagem', -, -, -]</t>
+          <t>MEC-3A-Fresagem</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-M. A. Comp; Cad / CAM', -]</t>
+          <t>MEC-3A-Fresagem</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[-, 'MEC-3A-M. A. Comp; Cad / CAM', -, -]</t>
+          <t>MEC-3A-Fresagem</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -894,7 +894,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[-, -, -, 'MEC-3A-Fresagem']</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
+          <t>MEC-3A-M. A. Comp; Cad / CAM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MEC-3A-M. A. Comp; Cad / CAM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[-, -, 'MEC-3A-Fresagem', -]</t>
+          <t>MEC-3A-M. A. Comp; Cad / CAM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>